<commit_message>
arregle el generador de sudokus
</commit_message>
<xml_diff>
--- a/crear sudokus.xlsx
+++ b/crear sudokus.xlsx
@@ -1,22 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julianmanera/Desktop/Programacion/SUDOKU/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAC91F8-6321-DB46-85C3-7A845918B7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="10515" windowHeight="3930" tabRatio="281"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="281" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="167">
   <si>
     <t>81--45---</t>
   </si>
@@ -468,14 +487,62 @@
     <t>387/491/625</t>
   </si>
   <si>
-    <t>"</t>
+    <t>763194582</t>
+  </si>
+  <si>
+    <t>192578634</t>
+  </si>
+  <si>
+    <t>814932756</t>
+  </si>
+  <si>
+    <t>375846129</t>
+  </si>
+  <si>
+    <t>629715348</t>
+  </si>
+  <si>
+    <t>256389417</t>
+  </si>
+  <si>
+    <t>981457263</t>
+  </si>
+  <si>
+    <t>437261895</t>
+  </si>
+  <si>
+    <t>SEGUNDA DISTRIBUCION</t>
+  </si>
+  <si>
+    <t>531648792</t>
+  </si>
+  <si>
+    <t>642759318</t>
+  </si>
+  <si>
+    <t>968412573</t>
+  </si>
+  <si>
+    <t>157983624</t>
+  </si>
+  <si>
+    <t>324567189</t>
+  </si>
+  <si>
+    <t>273194865</t>
+  </si>
+  <si>
+    <t>496875231</t>
+  </si>
+  <si>
+    <t>815236947</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,8 +555,21 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +579,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -618,41 +704,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,6 +757,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -710,7 +808,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -743,9 +841,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -778,6 +893,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -953,16 +1085,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AE24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AE15" sqref="AE15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>149</v>
       </c>
@@ -1009,11 +1155,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C5" s="1">
-        <v>387491625</v>
-      </c>
-      <c r="E5" s="6" t="s">
+    <row r="5" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G5" t="s">
@@ -1056,11 +1199,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
-        <v>241568379</v>
-      </c>
-      <c r="E6" s="6" t="s">
+    <row r="6" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G6" t="s">
@@ -1103,11 +1243,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
-        <v>569327418</v>
-      </c>
-      <c r="E7" s="6" t="s">
+    <row r="7" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G7" t="s">
@@ -1150,11 +1287,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
-        <v>758619234</v>
-      </c>
-      <c r="E8" s="6" t="s">
+    <row r="8" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G8" t="s">
@@ -1197,11 +1331,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
-        <v>123784596</v>
-      </c>
-      <c r="E9" s="6" t="s">
+    <row r="9" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G9" t="s">
@@ -1244,11 +1375,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
-        <v>496253187</v>
-      </c>
-      <c r="E10" s="6" t="s">
+    <row r="10" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
@@ -1291,11 +1419,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C11" s="1">
-        <v>934176852</v>
-      </c>
-      <c r="E11" s="6" t="s">
+    <row r="11" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G11" t="s">
@@ -1338,11 +1463,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C12" s="1">
-        <v>675832941</v>
-      </c>
-      <c r="E12" s="6" t="s">
+    <row r="12" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E12" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G12" t="s">
@@ -1385,11 +1507,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C13" s="1">
-        <v>812945763</v>
-      </c>
-      <c r="E13" s="6" t="s">
+    <row r="13" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="E13" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G13" t="s">
@@ -1432,51 +1551,164 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="3:31" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+    <row r="15" spans="3:31" ht="19" x14ac:dyDescent="0.25">
+      <c r="E15" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C16" s="1">
+        <v>387491625</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C17" s="1">
+        <v>241568379</v>
+      </c>
+      <c r="E17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" s="1">
+        <v>569327418</v>
+      </c>
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C19" s="1">
+        <v>758619234</v>
+      </c>
+      <c r="E19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C20" s="1">
+        <v>123784596</v>
+      </c>
+      <c r="E20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C21" s="1">
+        <v>496253187</v>
+      </c>
+      <c r="E21" t="s">
+        <v>154</v>
+      </c>
+      <c r="G21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C22" s="1">
+        <v>934176852</v>
+      </c>
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C23" s="1">
+        <v>675832941</v>
+      </c>
+      <c r="E23" t="s">
+        <v>156</v>
+      </c>
+      <c r="G23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C24" s="1">
+        <v>812945763</v>
+      </c>
+      <c r="E24" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="3:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="3:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="3:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
+      <c r="E31" s="17"/>
+    </row>
+    <row r="32" spans="3:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" spans="3:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" spans="3:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="3:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" spans="3:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C36" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C37" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1487,422 +1719,538 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:O12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C1:Q24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
       <selection activeCell="O3" sqref="O3:O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="3.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="2" customWidth="1"/>
-    <col min="7" max="13" width="3.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.83203125" style="2" customWidth="1"/>
+    <col min="7" max="13" width="3.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="3:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="4"/>
-      <c r="E3" s="7">
+    <row r="2" spans="5:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="5:17" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="10">
+        <v>7</v>
+      </c>
+      <c r="F3" s="11">
+        <v>8</v>
+      </c>
+      <c r="G3" s="12">
+        <v>9</v>
+      </c>
+      <c r="H3" s="13">
+        <v>3</v>
+      </c>
+      <c r="I3" s="11">
+        <v>2</v>
+      </c>
+      <c r="J3" s="14">
         <v>1</v>
       </c>
-      <c r="F3" s="10">
-        <v>9</v>
-      </c>
-      <c r="G3" s="8">
+      <c r="K3" s="12">
         <v>4</v>
       </c>
-      <c r="H3" s="11">
-        <v>8</v>
-      </c>
-      <c r="I3" s="10">
-        <v>2</v>
-      </c>
-      <c r="J3" s="12">
+      <c r="L3" s="11">
+        <v>5</v>
+      </c>
+      <c r="M3" s="15">
         <v>6</v>
       </c>
-      <c r="K3" s="8">
-        <v>3</v>
-      </c>
-      <c r="L3" s="10">
-        <v>5</v>
-      </c>
-      <c r="M3" s="15">
-        <v>7</v>
-      </c>
       <c r="O3" t="str">
-        <f>E3&amp;F3&amp;G3&amp;H3&amp;I3&amp;J3&amp;K3&amp;L3&amp;M3</f>
-        <v>194826357</v>
-      </c>
-    </row>
-    <row r="4" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="E4" s="4">
-        <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="F4" s="4">
+        <f t="shared" ref="O3:O11" si="0">E3&amp;F3&amp;G3&amp;H3&amp;I3&amp;J3&amp;K3&amp;L3&amp;M3</f>
+        <v>789321456</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="6">
         <f>L3</f>
         <v>5</v>
       </c>
-      <c r="G4" s="14">
+      <c r="F4" s="6">
+        <f>H3</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="7">
+        <f>J3</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
         <f>M3</f>
+        <v>6</v>
+      </c>
+      <c r="I4" s="6">
+        <f>K3</f>
+        <v>4</v>
+      </c>
+      <c r="J4" s="7">
+        <f>F3</f>
+        <v>8</v>
+      </c>
+      <c r="K4" s="6">
+        <f>E3</f>
         <v>7</v>
       </c>
-      <c r="H4" s="4">
-        <f>E3</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <f>F3</f>
+      <c r="L4" s="6">
+        <f>G3</f>
         <v>9</v>
       </c>
-      <c r="J4" s="14">
-        <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="K4" s="4">
-        <f>H3</f>
-        <v>8</v>
-      </c>
-      <c r="L4" s="4">
+      <c r="M4" s="6">
         <f>I3</f>
         <v>2</v>
       </c>
-      <c r="M4" s="4">
-        <f>J3</f>
+      <c r="O4" t="str">
+        <f t="shared" si="0"/>
+        <v>531648792</v>
+      </c>
+    </row>
+    <row r="5" spans="5:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="8">
+        <f>M3</f>
         <v>6</v>
       </c>
-      <c r="O4" t="str">
-        <f>E4&amp;F4&amp;G4&amp;H4&amp;I4&amp;J4&amp;K4&amp;L4&amp;M4</f>
-        <v>357194826</v>
-      </c>
-    </row>
-    <row r="5" spans="3:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
-      <c r="E5" s="9">
-        <f>H3</f>
-        <v>8</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
+        <f>K3</f>
+        <v>4</v>
+      </c>
+      <c r="G5" s="9">
         <f>I3</f>
         <v>2</v>
       </c>
-      <c r="G5" s="13">
-        <f>J3</f>
-        <v>6</v>
-      </c>
-      <c r="H5" s="9">
-        <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="H5" s="8">
+        <f>E3</f>
+        <v>7</v>
+      </c>
+      <c r="I5" s="8">
         <f>L3</f>
         <v>5</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="9">
+        <f>G3</f>
+        <v>9</v>
+      </c>
+      <c r="K5" s="8">
+        <f>H3</f>
+        <v>3</v>
+      </c>
+      <c r="L5" s="8">
+        <f>J3</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <f>F3</f>
+        <v>8</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="0"/>
+        <v>642759318</v>
+      </c>
+    </row>
+    <row r="6" spans="5:17" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="6">
+        <f>G3</f>
+        <v>9</v>
+      </c>
+      <c r="F6" s="6">
         <f>M3</f>
-        <v>7</v>
-      </c>
-      <c r="K5" s="9">
-        <f>E3</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="7">
+        <f>F3</f>
+        <v>8</v>
+      </c>
+      <c r="H6" s="6">
+        <f>K3</f>
+        <v>4</v>
+      </c>
+      <c r="I6" s="6">
+        <f>J3</f>
         <v>1</v>
       </c>
-      <c r="L5" s="9">
-        <f>F3</f>
-        <v>9</v>
-      </c>
-      <c r="M5" s="9">
-        <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="O5" t="str">
-        <f>E5&amp;F5&amp;G5&amp;H5&amp;I5&amp;J5&amp;K5&amp;L5&amp;M5</f>
-        <v>826357194</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="E6" s="4">
-        <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="F6" s="4">
-        <f>E3</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="14">
-        <f>F3</f>
-        <v>9</v>
-      </c>
-      <c r="H6" s="4">
-        <f>J3</f>
-        <v>6</v>
-      </c>
-      <c r="I6" s="4">
-        <f>H3</f>
-        <v>8</v>
-      </c>
-      <c r="J6" s="14">
+      <c r="J6" s="7">
         <f>I3</f>
         <v>2</v>
       </c>
-      <c r="K6" s="4">
-        <f>M3</f>
-        <v>7</v>
-      </c>
-      <c r="L6" s="4">
-        <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="M6" s="4">
+      <c r="K6" s="6">
         <f>L3</f>
         <v>5</v>
       </c>
+      <c r="L6" s="6">
+        <f>E3</f>
+        <v>7</v>
+      </c>
+      <c r="M6" s="6">
+        <f>H3</f>
+        <v>3</v>
+      </c>
       <c r="O6" t="str">
         <f>E6&amp;F6&amp;G6&amp;H6&amp;I6&amp;J6&amp;K6&amp;L6&amp;M6</f>
-        <v>419682735</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="E7" s="4">
-        <f>M3</f>
-        <v>7</v>
-      </c>
-      <c r="F7" s="4">
-        <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="G7" s="14">
+        <v>968412573</v>
+      </c>
+    </row>
+    <row r="7" spans="5:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E7" s="6">
+        <f>J3</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
         <f>L3</f>
         <v>5</v>
       </c>
-      <c r="H7" s="4">
+      <c r="G7" s="7">
+        <f>E3</f>
+        <v>7</v>
+      </c>
+      <c r="H7" s="6">
         <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="I7" s="4">
-        <f>E3</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="14">
+        <v>9</v>
+      </c>
+      <c r="I7" s="6">
         <f>F3</f>
-        <v>9</v>
-      </c>
-      <c r="K7" s="4">
-        <f>J3</f>
+        <v>8</v>
+      </c>
+      <c r="J7" s="7">
+        <f>H3</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="6">
+        <f>M3</f>
         <v>6</v>
       </c>
-      <c r="L7" s="4">
-        <f>H3</f>
-        <v>8</v>
-      </c>
-      <c r="M7" s="4">
+      <c r="L7" s="6">
         <f>I3</f>
         <v>2</v>
       </c>
+      <c r="M7" s="6">
+        <f>K3</f>
+        <v>4</v>
+      </c>
       <c r="O7" t="str">
-        <f>E7&amp;F7&amp;G7&amp;H7&amp;I7&amp;J7&amp;K7&amp;L7&amp;M7</f>
-        <v>735419682</v>
-      </c>
-    </row>
-    <row r="8" spans="3:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="E8" s="9">
-        <f>J3</f>
-        <v>6</v>
-      </c>
-      <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>157983624</v>
+      </c>
+    </row>
+    <row r="8" spans="5:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="8">
         <f>H3</f>
-        <v>8</v>
-      </c>
-      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="8">
         <f>I3</f>
         <v>2</v>
       </c>
-      <c r="H8" s="9">
-        <f>M3</f>
-        <v>7</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="G8" s="9">
         <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="J8" s="13">
+        <v>4</v>
+      </c>
+      <c r="H8" s="8">
         <f>L3</f>
         <v>5</v>
       </c>
-      <c r="K8" s="9">
+      <c r="I8" s="8">
+        <f>M3</f>
+        <v>6</v>
+      </c>
+      <c r="J8" s="9">
+        <f>E3</f>
+        <v>7</v>
+      </c>
+      <c r="K8" s="8">
+        <f>J3</f>
+        <v>1</v>
+      </c>
+      <c r="L8" s="8">
+        <f>F3</f>
+        <v>8</v>
+      </c>
+      <c r="M8" s="8">
         <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="L8" s="9">
-        <f>E3</f>
-        <v>1</v>
-      </c>
-      <c r="M8" s="9">
-        <f>F3</f>
         <v>9</v>
       </c>
-      <c r="N8" s="3"/>
       <c r="O8" t="str">
-        <f>E8&amp;F8&amp;G8&amp;H8&amp;I8&amp;J8&amp;K8&amp;L8&amp;M8</f>
-        <v>682735419</v>
-      </c>
-    </row>
-    <row r="9" spans="3:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
-      <c r="E9" s="4">
-        <f>F3</f>
-        <v>9</v>
-      </c>
-      <c r="F9" s="4">
-        <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="G9" s="14">
-        <f>E3</f>
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>324567189</v>
+      </c>
+    </row>
+    <row r="9" spans="5:17" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="6">
         <f>I3</f>
         <v>2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="F9" s="6">
+        <f>E3</f>
+        <v>7</v>
+      </c>
+      <c r="G9" s="7">
+        <f>H3</f>
+        <v>3</v>
+      </c>
+      <c r="H9" s="6">
         <f>J3</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <f>G3</f>
+        <v>9</v>
+      </c>
+      <c r="J9" s="7">
+        <f>K3</f>
+        <v>4</v>
+      </c>
+      <c r="K9" s="6">
+        <f>F3</f>
+        <v>8</v>
+      </c>
+      <c r="L9" s="6">
+        <f>M3</f>
         <v>6</v>
       </c>
-      <c r="J9" s="14">
-        <f>H3</f>
-        <v>8</v>
-      </c>
-      <c r="K9" s="4">
+      <c r="M9" s="6">
         <f>L3</f>
         <v>5</v>
       </c>
-      <c r="L9" s="4">
+      <c r="O9" t="str">
+        <f t="shared" si="0"/>
+        <v>273194865</v>
+      </c>
+    </row>
+    <row r="10" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E10" s="6">
+        <f>K3</f>
+        <v>4</v>
+      </c>
+      <c r="F10" s="6">
+        <f>G3</f>
+        <v>9</v>
+      </c>
+      <c r="G10" s="7">
         <f>M3</f>
+        <v>6</v>
+      </c>
+      <c r="H10" s="6">
+        <f>F3</f>
+        <v>8</v>
+      </c>
+      <c r="I10" s="6">
+        <f>E3</f>
         <v>7</v>
       </c>
-      <c r="M9" s="4">
-        <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="O9" t="str">
-        <f>E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9</f>
-        <v>941268573</v>
-      </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
-      <c r="E10" s="4">
+      <c r="J10" s="7">
         <f>L3</f>
         <v>5</v>
       </c>
-      <c r="F10" s="4">
-        <f>M3</f>
-        <v>7</v>
-      </c>
-      <c r="G10" s="14">
-        <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="H10" s="4">
-        <f>F3</f>
-        <v>9</v>
-      </c>
-      <c r="I10" s="4">
-        <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="J10" s="14">
-        <f>E3</f>
-        <v>1</v>
-      </c>
-      <c r="K10" s="4">
+      <c r="K10" s="6">
         <f>I3</f>
         <v>2</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="6">
+        <f>H3</f>
+        <v>3</v>
+      </c>
+      <c r="M10" s="6">
         <f>J3</f>
-        <v>6</v>
-      </c>
-      <c r="M10" s="4">
-        <f>H3</f>
+        <v>1</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="0"/>
+        <v>496875231</v>
+      </c>
+    </row>
+    <row r="11" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E11" s="6">
+        <f>F3</f>
         <v>8</v>
       </c>
-      <c r="O10" t="str">
-        <f>E10&amp;F10&amp;G10&amp;H10&amp;I10&amp;J10&amp;K10&amp;L10&amp;M10</f>
-        <v>573941268</v>
-      </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
-      <c r="E11" s="4">
+      <c r="F11" s="6">
+        <f>J3</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <f>L3</f>
+        <v>5</v>
+      </c>
+      <c r="H11" s="6">
         <f>I3</f>
         <v>2</v>
       </c>
-      <c r="F11" s="4">
-        <f>J3</f>
+      <c r="I11" s="6">
+        <f>H3</f>
+        <v>3</v>
+      </c>
+      <c r="J11" s="7">
+        <f>M3</f>
         <v>6</v>
       </c>
-      <c r="G11" s="14">
-        <f>H3</f>
-        <v>8</v>
-      </c>
-      <c r="H11" s="4">
-        <f>L3</f>
-        <v>5</v>
-      </c>
-      <c r="I11" s="4">
-        <f>M3</f>
+      <c r="K11" s="6">
+        <f>G3</f>
+        <v>9</v>
+      </c>
+      <c r="L11" s="6">
+        <f>K3</f>
+        <v>4</v>
+      </c>
+      <c r="M11" s="6">
+        <f>E3</f>
         <v>7</v>
       </c>
-      <c r="J11" s="14">
-        <f>K3</f>
-        <v>3</v>
-      </c>
-      <c r="K11" s="4">
-        <f>F3</f>
-        <v>9</v>
-      </c>
-      <c r="L11" s="4">
-        <f>G3</f>
-        <v>4</v>
-      </c>
-      <c r="M11" s="4">
-        <f>E3</f>
-        <v>1</v>
-      </c>
       <c r="O11" t="str">
-        <f>E11&amp;F11&amp;G11&amp;H11&amp;I11&amp;J11&amp;K11&amp;L11&amp;M11</f>
-        <v>268573941</v>
-      </c>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="G12" s="4"/>
+        <f t="shared" si="0"/>
+        <v>815236947</v>
+      </c>
+    </row>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="18"/>
+    </row>
+    <row r="16" spans="5:17" x14ac:dyDescent="0.2">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="18"/>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="18"/>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="18"/>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="18"/>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="18"/>
+    </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="18"/>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="18"/>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="18"/>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>